<commit_message>
Added time for comparison and new combobox
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -459,11 +459,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="306180736"/>
-        <c:axId val="147108240"/>
+        <c:axId val="146817112"/>
+        <c:axId val="146818680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="306180736"/>
+        <c:axId val="146817112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147108240"/>
+        <c:crossAx val="146818680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -570,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147108240"/>
+        <c:axId val="146818680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -659,7 +659,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -681,7 +681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306180736"/>
+        <c:crossAx val="146817112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Before submission report done, final version 2
</commit_message>
<xml_diff>
--- a/Comparison.xlsx
+++ b/Comparison.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NodesComputed" sheetId="1" r:id="rId1"/>
+    <sheet name="TimeRequired" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>N</t>
   </si>
@@ -23,6 +24,12 @@
   </si>
   <si>
     <t>Forward checking</t>
+  </si>
+  <si>
+    <t>Forward Checking with MRV</t>
+  </si>
+  <si>
+    <t>Minimum Conflicts</t>
   </si>
 </sst>
 </file>
@@ -112,11 +119,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Analysis: Number of nodes expanded for </a:t>
+              <a:t>Analysis</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>N-Queen puzzle </a:t>
+              <a:t> of nodes computed</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -154,7 +161,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2100531496062992"/>
+          <c:y val="0.16708333333333336"/>
+          <c:w val="0.75939129483814527"/>
+          <c:h val="0.51681284631087776"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -164,7 +181,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>NodesComputed!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -185,10 +202,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>NodesComputed!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -224,31 +241,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:f>NodesComputed!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>26</c:v>
                 </c:pt>
@@ -284,21 +286,6 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>20280</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>160712</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>91222</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>743229</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>48184</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3992510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,7 +296,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>NodesComputed!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -330,10 +317,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:f>NodesComputed!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -369,31 +356,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$18</c:f>
+              <c:f>NodesComputed!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -430,20 +402,235 @@
                 <c:pt idx="11">
                   <c:v>1360</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>10053</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5375</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41300</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2546</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>199636</c:v>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NodesComputed!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forward Checking with MRV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>NodesComputed!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NodesComputed!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NodesComputed!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minimum Conflicts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>NodesComputed!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NodesComputed!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,11 +646,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="146817112"/>
-        <c:axId val="146818680"/>
+        <c:axId val="367422528"/>
+        <c:axId val="367424096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146817112"/>
+        <c:axId val="367422528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,15 +749,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146818680"/>
+        <c:crossAx val="367424096"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146818680"/>
+        <c:axId val="367424096"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -612,8 +799,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Nodes Expanded</a:t>
+                  <a:t>Number of nodes computed</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in searh tree</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -659,14 +851,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -681,7 +870,931 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146817112"/>
+        <c:crossAx val="367422528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Analysis of time required</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeRequired!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Backtracking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeRequired!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeRequired!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeRequired!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forward checking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeRequired!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeRequired!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeRequired!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forward Checking with MRV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeRequired!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeRequired!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimeRequired!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minimum Conflicts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>TimeRequired!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimeRequired!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="146682888"/>
+        <c:axId val="146676224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="146682888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of queens</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146676224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="146676224"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in msec converted to log scale</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146682888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -802,6 +1915,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1305,24 +2458,562 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>566737</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1627,19 +3318,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1649,8 +3342,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1660,8 +3359,14 @@
       <c r="C2">
         <v>9</v>
       </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1671,8 +3376,14 @@
       <c r="C3">
         <v>6</v>
       </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1682,8 +3393,14 @@
       <c r="C4">
         <v>32</v>
       </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1693,8 +3410,14 @@
       <c r="C5">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1704,8 +3427,14 @@
       <c r="C6">
         <v>114</v>
       </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1715,8 +3444,14 @@
       <c r="C7">
         <v>42</v>
       </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1726,8 +3461,14 @@
       <c r="C8">
         <v>103</v>
       </c>
+      <c r="D8">
+        <v>49</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1737,8 +3478,14 @@
       <c r="C9">
         <v>53</v>
       </c>
+      <c r="D9">
+        <v>48</v>
+      </c>
+      <c r="E9">
+        <v>74</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1748,8 +3495,14 @@
       <c r="C10">
         <v>262</v>
       </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -1759,8 +3512,14 @@
       <c r="C11">
         <v>112</v>
       </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>56</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
@@ -1770,8 +3529,14 @@
       <c r="C12">
         <v>1900</v>
       </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>101</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -1781,60 +3546,11 @@
       <c r="C13">
         <v>1360</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>160712</v>
-      </c>
-      <c r="C14">
-        <v>10053</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>91222</v>
-      </c>
-      <c r="C15">
-        <v>5375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>743229</v>
-      </c>
-      <c r="C16">
-        <v>41300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>48184</v>
-      </c>
-      <c r="C17">
-        <v>2546</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>3992510</v>
-      </c>
-      <c r="C18">
-        <v>199636</v>
+      <c r="D13">
+        <v>47</v>
+      </c>
+      <c r="E13">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1842,4 +3558,298 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>137</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>114</v>
+      </c>
+      <c r="C15">
+        <v>503</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>193</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>